<commit_message>
fix(leveling): calculation of starting experience upon NPC and Player generation
</commit_message>
<xml_diff>
--- a/Data/leveling table.xlsx
+++ b/Data/leveling table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Serhii\EduProg\Mine\source\repos\gladiator-game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13753B4C-4800-4D8A-8B1A-D5C2423A10B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B0EB32-11E1-4471-A210-C61BFCC16DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -376,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>